<commit_message>
view last commit lol
</commit_message>
<xml_diff>
--- a/Notebooks/beispiel.xlsx
+++ b/Notebooks/beispiel.xlsx
@@ -464,17 +464,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>05.</t>
+          <t>05.Jan</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Jan</t>
+          <t>A</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>P1</t>
         </is>
       </c>
     </row>
@@ -486,17 +486,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>06.</t>
+          <t>06.Jan</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Jan</t>
+          <t>B</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>P3</t>
         </is>
       </c>
     </row>
@@ -508,17 +508,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>07.</t>
+          <t>07.Jan</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Jan</t>
+          <t>A</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>P1</t>
         </is>
       </c>
     </row>
@@ -530,17 +530,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>09.</t>
+          <t>09.Jan</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Jan</t>
+          <t>B</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>P2</t>
         </is>
       </c>
     </row>
@@ -552,17 +552,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>10.</t>
+          <t>10.Jan</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Jan</t>
+          <t>A</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>P3</t>
         </is>
       </c>
     </row>
@@ -574,17 +574,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>11.</t>
+          <t>11.Jan</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Jan</t>
+          <t>A</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>P2</t>
         </is>
       </c>
     </row>

</xml_diff>